<commit_message>
added negative cases validation for facebook
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/fbLoginCredentials.xlsx
+++ b/src/test/resources/testData/fbLoginCredentials.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Itonics\ItonicsAutomation\src\test\resources\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19455" windowHeight="7200"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15000" windowHeight="1740"/>
   </bookViews>
   <sheets>
     <sheet name="fbLoginCredentials" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,16 +34,16 @@
     <t>lastName</t>
   </si>
   <si>
-    <t>testing.facebook.automation@gmail.com</t>
-  </si>
-  <si>
     <t>reetik12345</t>
   </si>
   <si>
     <t>Adams</t>
   </si>
   <si>
-    <t>Lara</t>
+    <t>Lucy</t>
+  </si>
+  <si>
+    <t>testing.automate.facebook@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -379,7 +375,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,16 +396,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>